<commit_message>
logger added to main for demos. (inits)
</commit_message>
<xml_diff>
--- a/Booking/Booking_history.xlsx
+++ b/Booking/Booking_history.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CYTech Student\PycharmProjects\Quantitative_Finance\Booking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:80001_{ACA43921-64D2-4F61-9EBC-40341DEF6130}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:80001_{5EE7C9B8-E61C-4A5E-B698-107541E8CB36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="my_position" sheetId="1" r:id="rId1"/>
@@ -183,10 +183,10 @@
     <t>date</t>
   </si>
   <si>
-    <t>sp option</t>
-  </si>
-  <si>
-    <t>sp hedge</t>
+    <t>pnl option</t>
+  </si>
+  <si>
+    <t>pnl hedge</t>
   </si>
 </sst>
 </file>
@@ -606,7 +606,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="CYTech Student" refreshedDate="45558.888395833332" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="16" xr:uid="{00000000-000A-0000-FFFF-FFFF03000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="CYTech Student" refreshedDate="45609.508918402775" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="16" xr:uid="{00000000-000A-0000-FFFF-FFFF03000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:E1048576" sheet="histo_order"/>
   </cacheSource>
@@ -1169,11 +1169,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
@@ -2044,7 +2048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
demo added. logger issue fixed. volatility surface implementation.
</commit_message>
<xml_diff>
--- a/Booking/Booking_history.xlsx
+++ b/Booking/Booking_history.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CYTech Student\PycharmProjects\Quantitative_Finance\Booking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:80001_{5EE7C9B8-E61C-4A5E-B698-107541E8CB36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:80001_{775005D6-486E-40B7-9065-48E314818D50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="51">
   <si>
     <t>Étiquettes de lignes</t>
   </si>
@@ -181,12 +181,6 @@
   </si>
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>pnl option</t>
-  </si>
-  <si>
-    <t>pnl hedge</t>
   </si>
 </sst>
 </file>
@@ -606,7 +600,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="CYTech Student" refreshedDate="45609.508918402775" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="16" xr:uid="{00000000-000A-0000-FFFF-FFFF03000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="CYTech Student" refreshedDate="45617.528440393522" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="16" xr:uid="{00000000-000A-0000-FFFF-FFFF03000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:E1048576" sheet="histo_order"/>
   </cacheSource>
@@ -1167,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11:M12"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,30 +1725,6 @@
         <v>-4.8301088106938997E-3</v>
       </c>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H21" t="s">
-        <v>51</v>
-      </c>
-      <c r="I21">
-        <f>SUM(H2,H4,H16)</f>
-        <v>10057.33083415134</v>
-      </c>
-    </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H22" t="s">
-        <v>52</v>
-      </c>
-      <c r="I22">
-        <f>SUM(H3,H5:H15)</f>
-        <v>-9750</v>
-      </c>
-    </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="I23">
-        <f>SUM(I21:I22)</f>
-        <v>307.33083415134024</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1765,7 +1735,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>